<commit_message>
add instruction, add separate file used in psychopy by language
</commit_message>
<xml_diff>
--- a/letterlang test/letterorder_en.xlsx
+++ b/letterlang test/letterorder_en.xlsx
@@ -473,19 +473,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>letter/lettkh055.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettkh155.png</t>
         </is>
       </c>
     </row>
@@ -494,22 +494,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/lettth142.png</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/letten181.png</t>
         </is>
       </c>
     </row>
@@ -524,16 +524,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/letten181.png</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>letter/lettth132.png</t>
+          <t>letter/lettth142.png</t>
         </is>
       </c>
     </row>
@@ -548,16 +548,16 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>letter/lettkh013.png</t>
+          <t>letter/lettkh035.png</t>
         </is>
       </c>
     </row>
@@ -566,22 +566,22 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>letter/lettkh092.png</t>
+          <t>letter/lettgr061.png</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -590,22 +590,22 @@
         <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>letter/lettth101.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettgr065.png</t>
         </is>
       </c>
     </row>
@@ -614,22 +614,22 @@
         <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/letten112.png</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/lettkh083.png</t>
         </is>
       </c>
     </row>
@@ -638,22 +638,22 @@
         <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/letten041.png</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
     </row>
@@ -662,22 +662,22 @@
         <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>letter/lettkh091.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettgr066.png</t>
         </is>
       </c>
     </row>
@@ -689,19 +689,19 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>letter/letten153.png</t>
+          <t>letter/lettkh155.png</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>letter/lettkh159.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -713,19 +713,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>letter/lettth142.png</t>
+          <t>letter/letten091.png</t>
         </is>
       </c>
     </row>
@@ -740,16 +740,16 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>letter/lettkh013.png</t>
+          <t>letter/lettkh157.png</t>
         </is>
       </c>
     </row>
@@ -764,16 +764,16 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>letter/letten021.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>letter/lettgr021.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
     </row>
@@ -788,16 +788,16 @@
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>letter/lettkh034.png</t>
+          <t>letter/lettkh035.png</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
     </row>
@@ -809,19 +809,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>letter/lettth152.png</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>letter/letten142.png</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>letter/lettth152.png</t>
         </is>
       </c>
     </row>
@@ -836,16 +836,16 @@
         <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>letter/lettkh157.png</t>
+          <t>letter/lettkh155.png</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>letter/letten051.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -864,12 +864,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/letten021.png</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>letter/lettgr066.png</t>
+          <t>letter/lettgr021.png</t>
         </is>
       </c>
     </row>
@@ -878,22 +878,22 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>letter/lettkh055.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
     </row>
@@ -902,22 +902,22 @@
         <v>2</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>letter/letten161.png</t>
+          <t>letter/letten153.png</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>letter/lettgr161.png</t>
+          <t>letter/lettkh159.png</t>
         </is>
       </c>
     </row>
@@ -929,19 +929,19 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>letter/lettth101.png</t>
+          <t>letter/letten091.png</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
         <v>2</v>
@@ -960,12 +960,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/lettgr012.png</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/letten011.png</t>
         </is>
       </c>
     </row>
@@ -974,22 +974,22 @@
         <v>2</v>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>letter/letten021.png</t>
+          <t>letter/letten181.png</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>letter/lettgr021.png</t>
+          <t>letter/lettth142.png</t>
         </is>
       </c>
     </row>
@@ -998,22 +998,22 @@
         <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/lettkh157.png</t>
         </is>
       </c>
     </row>
@@ -1022,22 +1022,22 @@
         <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>letter/letten051.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>letter/lettkh157.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
     </row>
@@ -1052,11 +1052,11 @@
         <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>letter/lettgr061.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1073,19 +1073,19 @@
         <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/lettkh157.png</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>letter/lettkh092.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
     </row>
@@ -1100,16 +1100,16 @@
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/letten011.png</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/lettgr012.png</t>
         </is>
       </c>
     </row>
@@ -1118,22 +1118,22 @@
         <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/letten021.png</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettgr021.png</t>
         </is>
       </c>
     </row>
@@ -1142,22 +1142,22 @@
         <v>2</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>letter/lettgr092.png</t>
+          <t>letter/lettkh035.png</t>
         </is>
       </c>
     </row>
@@ -1166,22 +1166,22 @@
         <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>letter/lettth132.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
     </row>
@@ -1193,19 +1193,19 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>letter/lettth142.png</t>
+          <t>letter/letten131.png</t>
         </is>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
@@ -1224,12 +1224,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/letten153.png</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>letter/lettgr066.png</t>
+          <t>letter/lettkh159.png</t>
         </is>
       </c>
     </row>
@@ -1238,22 +1238,22 @@
         <v>2</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>letter/lettth142.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettkh055.png</t>
         </is>
       </c>
     </row>
@@ -1262,22 +1262,22 @@
         <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>letter/lettkh034.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettth101.png</t>
         </is>
       </c>
     </row>
@@ -1286,22 +1286,22 @@
         <v>2</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
         <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>letter/lettth132.png</t>
+          <t>letter/lettkh055.png</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
     </row>
@@ -1313,19 +1313,19 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>letter/lettth022.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>letter/letten041.png</t>
+          <t>letter/lettth101.png</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" t="n">
         <v>2</v>
@@ -1344,12 +1344,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>letter/lettgr152.png</t>
+          <t>letter/lettkh091.png</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>letter/letten151.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1382,22 +1382,22 @@
         <v>2</v>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>letter/lettkh155.png</t>
+          <t>letter/letten101.png</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/lettth011.png</t>
         </is>
       </c>
     </row>
@@ -1406,22 +1406,22 @@
         <v>2</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
         <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>letter/lettth011.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>letter/letten101.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -1430,22 +1430,22 @@
         <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>letter/lettkh013.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettgr061.png</t>
         </is>
       </c>
     </row>
@@ -1454,22 +1454,22 @@
         <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>letter/letten041.png</t>
+          <t>letter/lettkh083.png</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>letter/lettth022.png</t>
+          <t>letter/letten112.png</t>
         </is>
       </c>
     </row>
@@ -1484,7 +1484,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1505,19 +1505,19 @@
         <v>2</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>letter/lettkh159.png</t>
+          <t>letter/letten112.png</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>letter/letten153.png</t>
+          <t>letter/lettkh083.png</t>
         </is>
       </c>
     </row>
@@ -1526,22 +1526,22 @@
         <v>2</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
         <v>3</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>letter/letten041.png</t>
+          <t>letter/lettkh091.png</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>letter/lettth022.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1574,22 +1574,22 @@
         <v>2</v>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettth152.png</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>letter/lettkh091.png</t>
+          <t>letter/letten142.png</t>
         </is>
       </c>
     </row>
@@ -1598,22 +1598,22 @@
         <v>2</v>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/lettkh013.png</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>letter/lettgr092.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
     </row>
@@ -1622,22 +1622,22 @@
         <v>2</v>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>letter/letten151.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>letter/lettgr152.png</t>
+          <t>letter/letten091.png</t>
         </is>
       </c>
     </row>
@@ -1649,19 +1649,19 @@
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>letter/letten101.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>letter/lettth011.png</t>
+          <t>letter/letten041.png</t>
         </is>
       </c>
     </row>
@@ -1670,22 +1670,22 @@
         <v>2</v>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
         <v>3</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>letter/lettgr152.png</t>
+          <t>letter/letten142.png</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>letter/letten151.png</t>
+          <t>letter/lettth152.png</t>
         </is>
       </c>
     </row>
@@ -1694,22 +1694,22 @@
         <v>2</v>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>letter/letten051.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>letter/lettkh157.png</t>
+          <t>letter/letten131.png</t>
         </is>
       </c>
     </row>
@@ -1718,22 +1718,22 @@
         <v>2</v>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="n">
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>letter/lettgr061.png</t>
+          <t>letter/lettkh013.png</t>
         </is>
       </c>
     </row>
@@ -1742,22 +1742,22 @@
         <v>2</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>letter/lettth022.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>letter/letten041.png</t>
+          <t>letter/lettgr061.png</t>
         </is>
       </c>
     </row>
@@ -1766,22 +1766,22 @@
         <v>2</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettkh159.png</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/letten153.png</t>
         </is>
       </c>
     </row>
@@ -1790,22 +1790,22 @@
         <v>2</v>
       </c>
       <c r="B57" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/letten101.png</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>letter/lettgr061.png</t>
+          <t>letter/lettth011.png</t>
         </is>
       </c>
     </row>
@@ -1814,22 +1814,22 @@
         <v>2</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C58" t="n">
         <v>1</v>
       </c>
       <c r="D58" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>letter/letten171.png</t>
+          <t>letter/letten152.png</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>letter/lettth154.png</t>
+          <t>letter/lettgr152.png</t>
         </is>
       </c>
     </row>
@@ -1838,22 +1838,22 @@
         <v>2</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/lettgr021.png</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>letter/lettth132.png</t>
+          <t>letter/letten021.png</t>
         </is>
       </c>
     </row>
@@ -1868,16 +1868,16 @@
         <v>2</v>
       </c>
       <c r="D60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>letter/lettth011.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>letter/letten101.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -1886,22 +1886,22 @@
         <v>2</v>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" t="n">
         <v>2</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettgr061.png</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>letter/lettkh034.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -1910,22 +1910,22 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettkh055.png</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>letter/lettth101.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
     </row>
@@ -1934,22 +1934,22 @@
         <v>2</v>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/lettth101.png</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
     </row>
@@ -1958,22 +1958,22 @@
         <v>2</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
         <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/letten152.png</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/lettgr152.png</t>
         </is>
       </c>
     </row>
@@ -1982,17 +1982,17 @@
         <v>2</v>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
         <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>letter/lettkh013.png</t>
+          <t>letter/lettth101.png</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2012,16 +2012,16 @@
         <v>2</v>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>letter/lettgr092.png</t>
+          <t>letter/lettgr152.png</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/letten152.png</t>
         </is>
       </c>
     </row>
@@ -2033,19 +2033,19 @@
         <v>2</v>
       </c>
       <c r="C67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>letter/lettkh155.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/lettkh013.png</t>
         </is>
       </c>
     </row>
@@ -2060,16 +2060,16 @@
         <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>letter/letten161.png</t>
+          <t>letter/letten011.png</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>letter/lettgr161.png</t>
+          <t>letter/lettgr012.png</t>
         </is>
       </c>
     </row>
@@ -2078,22 +2078,22 @@
         <v>2</v>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>letter/lettgr066.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/lettkh091.png</t>
         </is>
       </c>
     </row>
@@ -2102,22 +2102,22 @@
         <v>2</v>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>letter/lettgr021.png</t>
+          <t>letter/letten131.png</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>letter/letten021.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
     </row>
@@ -2126,22 +2126,22 @@
         <v>2</v>
       </c>
       <c r="B71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>letter/lettkh055.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -2150,22 +2150,22 @@
         <v>2</v>
       </c>
       <c r="B72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>letter/lettkh159.png</t>
+          <t>letter/letten091.png</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>letter/letten153.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
     </row>
@@ -2180,16 +2180,16 @@
         <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>letter/lettgr092.png</t>
+          <t>letter/lettgr063.png</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>letter/letten091.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -2198,22 +2198,22 @@
         <v>2</v>
       </c>
       <c r="B74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74" t="n">
         <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>letter/lettth154.png</t>
+          <t>letter/lettgr066.png</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>letter/letten171.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -2222,22 +2222,22 @@
         <v>2</v>
       </c>
       <c r="B75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>letter/letten153.png</t>
+          <t>letter/lettgr065.png</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>letter/lettkh159.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -2249,19 +2249,19 @@
         <v>2</v>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/lettkh013.png</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>letter/lettkh092.png</t>
+          <t>letter/letten121.png</t>
         </is>
       </c>
     </row>
@@ -2276,16 +2276,16 @@
         <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>letter/lettgr161.png</t>
+          <t>letter/lettgr065.png</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>letter/letten161.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -2294,22 +2294,22 @@
         <v>2</v>
       </c>
       <c r="B78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" t="n">
         <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>letter/lettgr061.png</t>
+          <t>letter/lettkh083.png</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/letten112.png</t>
         </is>
       </c>
     </row>
@@ -2318,22 +2318,22 @@
         <v>2</v>
       </c>
       <c r="B79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/lettgr152.png</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>letter/lettkh091.png</t>
+          <t>letter/letten152.png</t>
         </is>
       </c>
     </row>
@@ -2348,16 +2348,16 @@
         <v>2</v>
       </c>
       <c r="D80" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>letter/lettth154.png</t>
+          <t>letter/lettth011.png</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>letter/letten171.png</t>
+          <t>letter/letten101.png</t>
         </is>
       </c>
     </row>
@@ -2366,22 +2366,22 @@
         <v>2</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>letter/letten101.png</t>
+          <t>letter/lettgr021.png</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>letter/lettth011.png</t>
+          <t>letter/letten021.png</t>
         </is>
       </c>
     </row>
@@ -2396,7 +2396,7 @@
         <v>2</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
     </row>
@@ -2414,22 +2414,22 @@
         <v>2</v>
       </c>
       <c r="B83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83" t="n">
         <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>letter/lettgr161.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>letter/letten161.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
     </row>
@@ -2441,19 +2441,19 @@
         <v>2</v>
       </c>
       <c r="C84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>letter/lettkh092.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/lettkh055.png</t>
         </is>
       </c>
     </row>
@@ -2465,19 +2465,19 @@
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>letter/letten171.png</t>
+          <t>letter/lettth011.png</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>letter/lettth154.png</t>
+          <t>letter/letten101.png</t>
         </is>
       </c>
     </row>
@@ -2492,16 +2492,16 @@
         <v>1</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
     </row>
@@ -2513,19 +2513,19 @@
         <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" t="n">
         <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/letten041.png</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>letter/letten181.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
     </row>
@@ -2534,13 +2534,13 @@
         <v>2</v>
       </c>
       <c r="B88" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
         <v>1</v>
       </c>
       <c r="D88" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/lettth132.png</t>
         </is>
       </c>
     </row>
@@ -2561,19 +2561,19 @@
         <v>3</v>
       </c>
       <c r="C89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>letter/lettgr063.png</t>
+          <t>letter/letten061.png</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>letter/letten062.png</t>
+          <t>letter/lettgr066.png</t>
         </is>
       </c>
     </row>
@@ -2582,22 +2582,22 @@
         <v>2</v>
       </c>
       <c r="B90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C90" t="n">
         <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/letten142.png</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>letter/lettkh055.png</t>
+          <t>letter/lettth152.png</t>
         </is>
       </c>
     </row>
@@ -2606,22 +2606,22 @@
         <v>2</v>
       </c>
       <c r="B91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>letter/letten061.png</t>
+          <t>letter/lettgr012.png</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>letter/lettkh155.png</t>
+          <t>letter/letten011.png</t>
         </is>
       </c>
     </row>
@@ -2633,19 +2633,19 @@
         <v>2</v>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/lettkh035.png</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>letter/lettkh034.png</t>
+          <t>letter/letten051.png</t>
         </is>
       </c>
     </row>
@@ -2654,22 +2654,22 @@
         <v>2</v>
       </c>
       <c r="B93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C93" t="n">
         <v>1</v>
       </c>
       <c r="D93" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>letter/letten151.png</t>
+          <t>letter/letten131.png</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>letter/lettgr152.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
     </row>
@@ -2678,22 +2678,22 @@
         <v>2</v>
       </c>
       <c r="B94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
         <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>letter/lettkh091.png</t>
+          <t>letter/lettth022.png</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>letter/letten071.png</t>
+          <t>letter/letten041.png</t>
         </is>
       </c>
     </row>
@@ -2705,19 +2705,19 @@
         <v>3</v>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>letter/lettgr021.png</t>
+          <t>letter/letten062.png</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>letter/letten021.png</t>
+          <t>letter/lettgr065.png</t>
         </is>
       </c>
     </row>
@@ -2726,22 +2726,22 @@
         <v>2</v>
       </c>
       <c r="B96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
         <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>letter/letten121.png</t>
+          <t>letter/letten071.png</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>letter/lettth101.png</t>
+          <t>letter/lettkh091.png</t>
         </is>
       </c>
     </row>
@@ -2750,22 +2750,22 @@
         <v>2</v>
       </c>
       <c r="B97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C97" t="n">
         <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>letter/lettth152.png</t>
+          <t>letter/lettkh159.png</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>letter/letten142.png</t>
+          <t>letter/letten153.png</t>
         </is>
       </c>
     </row>

</xml_diff>